<commit_message>
Creando estadisticas... los arqueros se han roto
He añadido el Promise.all a las peleas para asegurarme que todas se ejecutan.
</commit_message>
<xml_diff>
--- a/estadisticas.xlsx
+++ b/estadisticas.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="2808" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="numPVPs">Hoja1!$L$3</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,40 +22,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Archer</t>
-  </si>
-  <si>
-    <t>Berserker</t>
-  </si>
-  <si>
-    <t>Deffender</t>
-  </si>
-  <si>
-    <t>fencers</t>
-  </si>
-  <si>
-    <t>Ninja</t>
-  </si>
-  <si>
-    <t>Paladin</t>
-  </si>
-  <si>
-    <t>Sniper</t>
-  </si>
-  <si>
-    <t>Soldier</t>
-  </si>
-  <si>
-    <t>Thieve</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
+  <si>
+    <t>1 archer</t>
+  </si>
+  <si>
+    <t>2 berserk</t>
+  </si>
+  <si>
+    <t>3 defender</t>
+  </si>
+  <si>
+    <t>4 fencer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 ninja </t>
+  </si>
+  <si>
+    <t>6 paladin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 sniper </t>
+  </si>
+  <si>
+    <t>8 soldier</t>
+  </si>
+  <si>
+    <t>9 thieves</t>
+  </si>
+  <si>
+    <t>5 ninja</t>
+  </si>
+  <si>
+    <t>7 sniper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la Row  dice cuantos han vencido. Ej: la row del defensor dice cuantos ha vencido. Ergo la columna dice cuantas veces ha perdido. </t>
+  </si>
+  <si>
+    <t>5c y 4d son complementarios. La suma - 1000 es el numero de empates.</t>
+  </si>
+  <si>
+    <t>Num Combates probados:</t>
+  </si>
+  <si>
+    <t>Empates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +84,86 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,17 +175,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -366,161 +476,567 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J26"/>
+  <dimension ref="A2:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="10" width="16.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="K2" s="11"/>
+      <c r="L2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3">
+        <v>953</v>
+      </c>
+      <c r="L3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>65</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4">
+        <v>140</v>
+      </c>
+      <c r="E4">
+        <v>522</v>
+      </c>
+      <c r="F4">
+        <v>595</v>
+      </c>
+      <c r="G4">
+        <v>491</v>
+      </c>
+      <c r="H4">
+        <v>561</v>
+      </c>
+      <c r="I4">
+        <v>605</v>
+      </c>
+      <c r="J4">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>933</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>539</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="C7">
+        <v>472</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>559</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>441</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>445</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>262</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="D15" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="E15" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="F15" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="G15" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="H15" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="I15" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="J15" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="10">
+        <f ca="1">C2:C25</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
+        <f>B4/C3</f>
+        <v>6.8205666316894023E-2</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5">
+        <v>522</v>
+      </c>
+      <c r="F17" s="5">
+        <v>595</v>
+      </c>
+      <c r="G17" s="5">
+        <v>491</v>
+      </c>
+      <c r="H17" s="5">
+        <v>561</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5">
+        <v>933</v>
+      </c>
+      <c r="D18" s="5">
+        <v>140</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5">
+        <v>539</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5">
+        <v>472</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5">
+        <v>559</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5">
+        <v>441</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+      <c r="B27" s="7"/>
+      <c r="C27" s="10">
+        <f>B4+C3-1000</f>
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <f>B5+D3-numPVPs</f>
+        <v>-1000</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="12">
+        <f>B4+C3-numPVPs</f>
+        <v>18</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="5">
+        <f>D4+C5-numPVPs</f>
+        <v>73</v>
+      </c>
+      <c r="E28" s="5">
+        <f>E4+C6-numPVPs</f>
+        <v>61</v>
+      </c>
+      <c r="F28" s="5">
+        <f>F4+C7-numPVPs</f>
+        <v>67</v>
+      </c>
+      <c r="G28" s="5">
+        <f>G4+C8-numPVPs</f>
+        <v>50</v>
+      </c>
+      <c r="H28" s="5">
+        <f>H4+C9-numPVPs</f>
         <v>2</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+      <c r="I28" s="5">
+        <f>I4+C10-numPVPs</f>
+        <v>50</v>
+      </c>
+      <c r="J28" s="5">
+        <f>J4+C11-numPVPs</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5">
+        <f>D4+C5-numPVPs</f>
+        <v>73</v>
+      </c>
+      <c r="D29" s="5">
+        <v>140</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5">
+        <f>E4+C6-numPVPs</f>
+        <v>61</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5">
+        <f>F4+C7-numPVPs</f>
+        <v>67</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5">
+        <f>G4+C8-numPVPs</f>
+        <v>50</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5">
+        <f>H4+C9-numPVPs</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="1">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="1">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="1">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="1">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="1">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5">
+        <f>I4+C10-numPVPs</f>
+        <v>50</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="1">
-        <v>9</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5">
+        <f>J4+C11-numPVPs</f>
+        <v>2</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>